<commit_message>
Merging Narendra's and Rajdeep's code
</commit_message>
<xml_diff>
--- a/src/test/resources/com/aem/datasource/TestSuite.xlsx
+++ b/src/test/resources/com/aem/datasource/TestSuite.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="4908" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
     <sheet name="Test Steps" sheetId="1" r:id="rId2"/>
-    <sheet name="Test Data" sheetId="3" r:id="rId3"/>
-    <sheet name="Settings" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Test Data" sheetId="3" r:id="rId4"/>
+    <sheet name="Settings" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Action_Keywords">Settings!$D$2:$D$8</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="145">
   <si>
     <t>Description</t>
   </si>
@@ -79,18 +80,6 @@
     <t>Test@123</t>
   </si>
   <si>
-    <t>Click on My Account button on the Top Right location</t>
-  </si>
-  <si>
-    <t>Enter the Username in the UserName field</t>
-  </si>
-  <si>
-    <t>Click on Login button</t>
-  </si>
-  <si>
-    <t>Close the Browser</t>
-  </si>
-  <si>
     <t>Open the Browser</t>
   </si>
   <si>
@@ -148,15 +137,6 @@
     <t>LogIn_Page</t>
   </si>
   <si>
-    <t>Wait for Some time</t>
-  </si>
-  <si>
-    <t>Click on LogOut button</t>
-  </si>
-  <si>
-    <t>Enter the Password in the Password field</t>
-  </si>
-  <si>
     <t>Page Object</t>
   </si>
   <si>
@@ -178,43 +158,307 @@
     <t>Verify Home Page</t>
   </si>
   <si>
-    <t>Login in to the Online Store Application</t>
-  </si>
-  <si>
     <t>Verify contents of home page</t>
   </si>
   <si>
-    <t>Verify Login</t>
-  </si>
-  <si>
-    <t>Open application</t>
-  </si>
-  <si>
-    <t>btn_CloseWindow</t>
-  </si>
-  <si>
-    <t>http://www.makemytrip.com/</t>
-  </si>
-  <si>
-    <t>http://www.store.demoqa.com</t>
-  </si>
-  <si>
-    <t>Navigate to store website</t>
-  </si>
-  <si>
-    <t>Navigate to make my trip website</t>
-  </si>
-  <si>
     <t>TS_003</t>
   </si>
   <si>
     <t>TS_008</t>
   </si>
   <si>
+    <t>Edit Profile Headers</t>
+  </si>
+  <si>
+    <t>Edit the profile headers in author instance</t>
+  </si>
+  <si>
+    <t>http://tour-asp-daut1.syd.aws.haylix.net:4502/cf#/en-gb/secure/profile.html</t>
+  </si>
+  <si>
+    <t>btn_Edit</t>
+  </si>
+  <si>
+    <t>txtbx_PersonalInfo</t>
+  </si>
+  <si>
+    <t>Edit Component</t>
+  </si>
+  <si>
+    <t>Enter Personal Info Header name</t>
+  </si>
+  <si>
+    <t>Enter Company Info Header name</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>btn_SignIn</t>
+  </si>
+  <si>
+    <t>txtbx_Username</t>
+  </si>
+  <si>
+    <t>Enter Username</t>
+  </si>
+  <si>
+    <t>Enter Password</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>dchandra</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Navigate to TA website</t>
+  </si>
+  <si>
+    <t>frame1</t>
+  </si>
+  <si>
+    <t>switchToFrame</t>
+  </si>
+  <si>
+    <t>Switch to the specified frame</t>
+  </si>
+  <si>
+    <t>TS_010</t>
+  </si>
+  <si>
+    <t>txtbx_CompanyInfo</t>
+  </si>
+  <si>
+    <t>btn_Ok</t>
+  </si>
+  <si>
+    <t>TS_011</t>
+  </si>
+  <si>
+    <t>Edit Hero Banner</t>
+  </si>
+  <si>
+    <t>Update Hero banner image for profiles</t>
+  </si>
+  <si>
+    <t>Confirm by clicking on ok button</t>
+  </si>
+  <si>
+    <t>TS_012</t>
+  </si>
+  <si>
+    <t>TS_013</t>
+  </si>
+  <si>
+    <t>btn_Search</t>
+  </si>
+  <si>
+    <t>element_AssetOption</t>
+  </si>
+  <si>
+    <t>btn_SearchOptionOk</t>
+  </si>
+  <si>
+    <t>Click on Search Option</t>
+  </si>
+  <si>
+    <t>Select Location</t>
+  </si>
+  <si>
+    <t>Confirm Selection</t>
+  </si>
+  <si>
+    <t>switchToDefaultContent</t>
+  </si>
+  <si>
+    <t>Switch to top window</t>
+  </si>
+  <si>
+    <t>tab_SideKickPages</t>
+  </si>
+  <si>
+    <t>Click on Pages tab in sidekick</t>
+  </si>
+  <si>
+    <t>tab_SideKickActivatePage</t>
+  </si>
+  <si>
+    <t>TS_014</t>
+  </si>
+  <si>
+    <t>TS_015</t>
+  </si>
+  <si>
+    <t>Click on Activate Page</t>
+  </si>
+  <si>
+    <t>Navigate to profiles page in publish instance</t>
+  </si>
+  <si>
+    <t>http://tour-asp-dpub1.syd.aws.haylix.net:4503/en-gb/secure/profile.html</t>
+  </si>
+  <si>
+    <t>txtbx_PublishUserName</t>
+  </si>
+  <si>
+    <t>lnk_SignIn</t>
+  </si>
+  <si>
+    <t>txtbx_PublishPassword</t>
+  </si>
+  <si>
+    <t>btn_PublishSignIn</t>
+  </si>
+  <si>
+    <t>TS_016</t>
+  </si>
+  <si>
+    <t>TS_017</t>
+  </si>
+  <si>
+    <t>TS_018</t>
+  </si>
+  <si>
+    <t>TS_019</t>
+  </si>
+  <si>
+    <t>TS_020</t>
+  </si>
+  <si>
+    <t>TS_021</t>
+  </si>
+  <si>
+    <t>getTextFromElementAndCompare</t>
+  </si>
+  <si>
+    <t>lbl_PublishPersonalInfo</t>
+  </si>
+  <si>
+    <t>lbl_PublishCompanyInfo</t>
+  </si>
+  <si>
+    <t>TS_022</t>
+  </si>
+  <si>
+    <t>TS_023</t>
+  </si>
+  <si>
+    <t>TS_024</t>
+  </si>
+  <si>
+    <t>TS_025</t>
+  </si>
+  <si>
+    <t>TS_026</t>
+  </si>
+  <si>
+    <t>TS_027</t>
+  </si>
+  <si>
+    <t>Publish Headers</t>
+  </si>
+  <si>
+    <t>Test publish</t>
+  </si>
+  <si>
+    <t>waitForPageToLoad</t>
+  </si>
+  <si>
+    <t>TS_028</t>
+  </si>
+  <si>
+    <t>Wait for five seconds</t>
+  </si>
+  <si>
+    <t>Click on Sign In link</t>
+  </si>
+  <si>
+    <t>Wait for page load</t>
+  </si>
+  <si>
+    <t>Click on Sign In button</t>
+  </si>
+  <si>
+    <t>Compare Personal information title</t>
+  </si>
+  <si>
+    <t>Compare Company information title</t>
+  </si>
+  <si>
+    <t>Drag And Drop Component</t>
+  </si>
+  <si>
+    <t>Verify drag and drop</t>
+  </si>
+  <si>
+    <t>sidekick_Expand</t>
+  </si>
+  <si>
+    <t>placeholder_AddComponent</t>
+  </si>
+  <si>
+    <t>doubleClick</t>
+  </si>
+  <si>
+    <t>Double click on the place holder to add the component</t>
+  </si>
+  <si>
+    <t>Click on expand button in the dialog present in the frame</t>
+  </si>
+  <si>
+    <t>comp_CertificateGenerator</t>
+  </si>
+  <si>
+    <t>btn_ComponentSelectionConfirmation</t>
+  </si>
+  <si>
+    <t>lbl_UserName</t>
+  </si>
+  <si>
+    <t>Verify name in the cerificate.</t>
+  </si>
+  <si>
+    <t>inputPassword</t>
+  </si>
+  <si>
+    <t>YWRtaW4=</t>
+  </si>
+  <si>
+    <t>Select Certificate Generator Component</t>
+  </si>
+  <si>
+    <t>Confirm Certificate Component Selection</t>
+  </si>
+  <si>
+    <t>Wait For 10 Seconds</t>
+  </si>
+  <si>
+    <t>Add Certificate Component in Author and verify the contents of certificate in publish environment</t>
+  </si>
+  <si>
+    <t>Add Cerificate Component</t>
+  </si>
+  <si>
+    <t>TS_029</t>
+  </si>
+  <si>
+    <t>TS_030</t>
+  </si>
+  <si>
+    <t>AARON JENNINGS</t>
+  </si>
+  <si>
+    <t>Personal Information</t>
+  </si>
+  <si>
+    <t>Company Information</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -307,7 +551,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -613,16 +857,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="D3" sqref="D3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="55.44140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="39.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="86.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -637,35 +881,83 @@
         <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -676,21 +968,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D42" workbookViewId="0">
+      <selection activeCell="G69" sqref="G68:G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="25.33203125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="48.44140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="66.33203125" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="11.0" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="38.109375" collapsed="true"/>
   </cols>
@@ -700,320 +992,1262 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
+      <c r="A2" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="H4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="2" t="str">
-        <f>'Test Data'!B2</f>
-        <v>testuser_3</v>
+        <v>132</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <f>'Test Data'!C2</f>
-        <v>Test@123</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
+      <c r="A7" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
+      <c r="A8" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
+      <c r="A9" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>53</v>
+      <c r="A10" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
+      <c r="C10" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>50</v>
+      <c r="A11" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G11" s="2"/>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>50</v>
+      <c r="A12" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2"/>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>50</v>
+      <c r="A13" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>74</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="2"/>
       <c r="H13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H57" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28:D33 D2:D7">
       <formula1>Page_Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3 F19 F28:F29 F48">
       <formula1>Action_Keywords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28:E33 E2:E7">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G12" r:id="rId2"/>
+    <hyperlink ref="G19" r:id="rId1"/>
+    <hyperlink ref="G48" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1021,6 +2255,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1044,26 +2290,26 @@
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -1072,7 +2318,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1120,7 +2366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1135,27 +2381,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -1163,13 +2409,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -1179,7 +2425,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
@@ -1190,7 +2436,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1206,7 +2452,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>